<commit_message>
Add invoicing periods bounds to example 06
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/06-long-term-planning-SA/06-long-term-planning-SA.xlsx
+++ b/ampl-data-input-excel/06-long-term-planning-SA/06-long-term-planning-SA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="15"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="experts" sheetId="1" state="visible" r:id="rId3"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="108">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -744,7 +744,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -787,8 +787,8 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -813,9 +813,18 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>200</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
@@ -1248,7 +1257,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -3966,7 +3975,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>